<commit_message>
Updated the program for Cross Over Design in TA and TE creation
</commit_message>
<xml_diff>
--- a/tests/testthat/STUDY003_TA.xlsx
+++ b/tests/testthat/STUDY003_TA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">STUDYID</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">ET3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHOUT</t>
   </si>
   <si>
     <t xml:space="preserve"> WASHOUT</t>
@@ -580,7 +583,7 @@
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -600,10 +603,10 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -628,7 +631,7 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
@@ -636,7 +639,7 @@
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -656,10 +659,10 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
@@ -675,16 +678,16 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -703,19 +706,19 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" t="n">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -731,16 +734,16 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" t="n">
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
         <v>19</v>
@@ -748,7 +751,7 @@
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -759,19 +762,19 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" t="n">
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -787,16 +790,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" t="n">
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
         <v>19</v>
@@ -804,7 +807,7 @@
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -815,16 +818,16 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" t="n">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
@@ -843,16 +846,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
@@ -871,19 +874,19 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E15" t="n">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -899,16 +902,16 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E16" t="n">
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G16" t="s">
         <v>19</v>
@@ -916,7 +919,7 @@
       <c r="H16"/>
       <c r="I16"/>
       <c r="J16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
@@ -927,16 +930,16 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E17" t="n">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G17" t="s">
         <v>16</v>
@@ -955,16 +958,16 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E18" t="n">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G18" t="s">
         <v>19</v>
@@ -972,7 +975,7 @@
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19">
@@ -983,19 +986,19 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E19" t="n">
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>

</xml_diff>